<commit_message>
add synthesis worksheet with draft terms applicable to samples
</commit_message>
<xml_diff>
--- a/notes/vocabulary/RoleVocabulary.xlsx
+++ b/notes/vocabulary/RoleVocabulary.xlsx
@@ -1,23 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GitHub\iSamples\metadata\vocabulary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GithubC\iSamples\metadata\notes\vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE342EF3-61FD-4FD9-90D8-C7F92F99DB26}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B627D58-173D-4019-A5C2-FA00A615D56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="900" yWindow="2715" windowWidth="27345" windowHeight="12990" activeTab="1" xr2:uid="{6D09EB57-77EB-4B90-8113-743A5CC7E14E}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="24060" windowHeight="15270" activeTab="2" xr2:uid="{6D09EB57-77EB-4B90-8113-743A5CC7E14E}"/>
   </bookViews>
   <sheets>
-    <sheet name="Roles" sheetId="1" r:id="rId1"/>
-    <sheet name="cessda-ddi roles" sheetId="2" r:id="rId2"/>
+    <sheet name="synthesis" sheetId="3" r:id="rId1"/>
+    <sheet name="Roles" sheetId="1" r:id="rId2"/>
+    <sheet name="cessda-ddi roles" sheetId="2" r:id="rId3"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Roles!$F$1:$F$128</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">Roles!$F$1:$F$128</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="309">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="319">
   <si>
     <t>Entry</t>
   </si>
@@ -966,13 +967,43 @@
   </si>
   <si>
     <t>DataProcessing. DataValidation</t>
+  </si>
+  <si>
+    <t>role</t>
+  </si>
+  <si>
+    <t>scope note</t>
+  </si>
+  <si>
+    <t>Who is responsible for providing access to  the sample (or part of it) for research</t>
+  </si>
+  <si>
+    <t>ISO19115-1, DataCite4.4</t>
+  </si>
+  <si>
+    <t>DataCredit, DataCite 4.4</t>
+  </si>
+  <si>
+    <t>DataCredit, casRAI,ISO19115-1, DataCite4.4</t>
+  </si>
+  <si>
+    <t>Role related to Initiative or Curation-- Leader of project that supported sample collection or curation activities</t>
+  </si>
+  <si>
+    <t>Role related to Initiative or Curation-- Manager of project that supported sample collection activities; might not be necessary</t>
+  </si>
+  <si>
+    <t>DataCredit, casRAI, DataCite4.4</t>
+  </si>
+  <si>
+    <t>Person on the membership list of a designated project/project team</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1030,6 +1061,12 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="3">
     <fill>
@@ -1077,24 +1114,24 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
@@ -1109,12 +1146,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
@@ -1124,14 +1155,11 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="1" applyFill="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
@@ -1451,11 +1479,162 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C4C688-E06A-402C-B8FF-1231BDDB6C39}">
-  <dimension ref="A1:F106"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8140B6-11ED-4C30-ABC1-8C066247C7B6}">
+  <dimension ref="A1:C12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B11" sqref="B11"/>
+      <selection activeCell="A12" sqref="A12:B12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="22.42578125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="65.7109375" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.42578125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="3"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="3" t="s">
+        <v>166</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>148</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="3" t="s">
+        <v>127</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>134</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>151</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>313</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="3" t="s">
+        <v>135</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>152</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>154</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="3" t="s">
+        <v>129</v>
+      </c>
+      <c r="B9" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="C9" s="3" t="s">
+        <v>317</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="3" t="s">
+        <v>128</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="B11" s="3" t="s">
+        <v>156</v>
+      </c>
+      <c r="C11" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A12" s="3" t="s">
+        <v>164</v>
+      </c>
+      <c r="B12" s="3" t="s">
+        <v>165</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="8" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C4C688-E06A-402C-B8FF-1231BDDB6C39}">
+  <dimension ref="A1:F99"/>
+  <sheetViews>
+    <sheetView topLeftCell="A72" workbookViewId="0">
+      <selection activeCell="A69" sqref="A69:B69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1477,24 +1656,24 @@
       <c r="B1" s="7" t="s">
         <v>147</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="D1" s="13" t="s">
+      <c r="D1" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="13" t="s">
+      <c r="F1" s="11" t="s">
         <v>87</v>
       </c>
     </row>
     <row r="2" spans="1:6" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="14" t="s">
+      <c r="A2" s="12" t="s">
         <v>166</v>
       </c>
-      <c r="B2" s="12" t="s">
+      <c r="B2" s="3" t="s">
         <v>148</v>
       </c>
       <c r="C2" s="1"/>
@@ -1503,8 +1682,7 @@
       <c r="F2" s="1"/>
     </row>
     <row r="3" spans="1:6" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="12"/>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="4" t="s">
         <v>137</v>
       </c>
       <c r="D3" s="3" t="s">
@@ -1516,7 +1694,6 @@
     </row>
     <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A4" s="2"/>
-      <c r="B4" s="12"/>
       <c r="C4" s="3" t="s">
         <v>28</v>
       </c>
@@ -1534,7 +1711,7 @@
       <c r="A5" s="7" t="s">
         <v>144</v>
       </c>
-      <c r="B5" s="12" t="s">
+      <c r="B5" s="3" t="s">
         <v>149</v>
       </c>
       <c r="C5" s="3"/>
@@ -1544,7 +1721,6 @@
       <c r="F5" s="2"/>
     </row>
     <row r="6" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="12"/>
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1557,7 +1733,6 @@
       </c>
     </row>
     <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
       <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1569,7 +1744,6 @@
       </c>
     </row>
     <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B8" s="12"/>
       <c r="C8" s="3" t="s">
         <v>81</v>
       </c>
@@ -1584,7 +1758,7 @@
       <c r="A9" s="9" t="s">
         <v>167</v>
       </c>
-      <c r="B9" s="12" t="s">
+      <c r="B9" s="3" t="s">
         <v>149</v>
       </c>
       <c r="C9" s="3" t="s">
@@ -1599,7 +1773,6 @@
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B10" s="12"/>
       <c r="C10" s="3"/>
       <c r="F10" s="5"/>
     </row>
@@ -1607,7 +1780,7 @@
       <c r="A11" s="10" t="s">
         <v>54</v>
       </c>
-      <c r="B11" s="12" t="s">
+      <c r="B11" s="3" t="s">
         <v>149</v>
       </c>
       <c r="C11" s="3" t="s">
@@ -1624,12 +1797,11 @@
       <c r="A12" s="8" t="s">
         <v>52</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="3" t="s">
         <v>149</v>
       </c>
     </row>
     <row r="13" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
@@ -1642,7 +1814,6 @@
       </c>
     </row>
     <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
-      <c r="B14" s="12"/>
       <c r="C14" s="3" t="s">
         <v>52</v>
       </c>
@@ -1654,7 +1825,6 @@
       </c>
     </row>
     <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
       <c r="C15" s="3" t="s">
         <v>82</v>
       </c>
@@ -1669,14 +1839,13 @@
       <c r="A16" s="8" t="s">
         <v>126</v>
       </c>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="3" t="s">
         <v>149</v>
       </c>
       <c r="C16" s="3"/>
       <c r="F16" s="2"/>
     </row>
     <row r="17" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
       <c r="C17" s="3" t="s">
         <v>77</v>
       </c>
@@ -1688,7 +1857,6 @@
       </c>
     </row>
     <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B18" s="12"/>
       <c r="C18" s="3" t="s">
         <v>77</v>
       </c>
@@ -1700,17 +1868,16 @@
       </c>
     </row>
     <row r="19" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A19" s="15" t="s">
+      <c r="A19" s="13" t="s">
         <v>127</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="3" t="s">
         <v>150</v>
       </c>
       <c r="C19" s="3"/>
       <c r="F19" s="6"/>
     </row>
     <row r="20" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B20" s="12"/>
       <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
@@ -1723,7 +1890,6 @@
       </c>
     </row>
     <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
       <c r="C21" s="3" t="s">
         <v>60</v>
       </c>
@@ -1735,7 +1901,6 @@
       </c>
     </row>
     <row r="22" spans="1:6" ht="150" x14ac:dyDescent="0.25">
-      <c r="B22" s="12"/>
       <c r="C22" s="3" t="s">
         <v>67</v>
       </c>
@@ -1747,17 +1912,16 @@
       </c>
     </row>
     <row r="23" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+      <c r="A23" s="13" t="s">
         <v>134</v>
       </c>
-      <c r="B23" s="12" t="s">
+      <c r="B23" s="3" t="s">
         <v>151</v>
       </c>
       <c r="C23" s="3"/>
       <c r="F23" s="2"/>
     </row>
     <row r="24" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="12"/>
       <c r="C24" s="3" t="s">
         <v>84</v>
       </c>
@@ -1769,7 +1933,6 @@
       </c>
     </row>
     <row r="25" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
       <c r="C25" s="3" t="s">
         <v>48</v>
       </c>
@@ -1781,16 +1944,15 @@
       </c>
     </row>
     <row r="26" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A26" s="15" t="s">
+      <c r="A26" s="13" t="s">
         <v>135</v>
       </c>
-      <c r="B26" s="12" t="s">
+      <c r="B26" s="3" t="s">
         <v>152</v>
       </c>
       <c r="C26" s="3"/>
     </row>
     <row r="27" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
       <c r="C27" s="3" t="s">
         <v>85</v>
       </c>
@@ -1802,7 +1964,6 @@
       </c>
     </row>
     <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B28" s="12"/>
       <c r="C28" s="3" t="s">
         <v>70</v>
       </c>
@@ -1814,7 +1975,6 @@
       </c>
     </row>
     <row r="29" spans="1:6" ht="240" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
       <c r="C29" s="3" t="s">
         <v>49</v>
       </c>
@@ -1826,7 +1986,6 @@
       </c>
     </row>
     <row r="30" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="B30" s="12"/>
       <c r="C30" s="3" t="s">
         <v>50</v>
       </c>
@@ -1838,7 +1997,6 @@
       </c>
     </row>
     <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
       <c r="C31" s="3" t="s">
         <v>12</v>
       </c>
@@ -1853,10 +2011,10 @@
       </c>
     </row>
     <row r="32" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="15" t="s">
+      <c r="A32" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B32" s="12" t="s">
+      <c r="B32" s="3" t="s">
         <v>153</v>
       </c>
       <c r="C32" s="3"/>
@@ -1864,7 +2022,6 @@
       <c r="F32" s="2"/>
     </row>
     <row r="33" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
       <c r="C33" s="3" t="s">
         <v>15</v>
       </c>
@@ -1877,7 +2034,6 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
-      <c r="B34" s="12"/>
       <c r="C34" s="3" t="s">
         <v>51</v>
       </c>
@@ -1889,7 +2045,6 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B35" s="12"/>
       <c r="C35" s="3" t="s">
         <v>38</v>
       </c>
@@ -1902,7 +2057,6 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="135" x14ac:dyDescent="0.25">
-      <c r="B36" s="12"/>
       <c r="C36" s="3" t="s">
         <v>53</v>
       </c>
@@ -1914,16 +2068,15 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="15" t="s">
+      <c r="A37" s="13" t="s">
         <v>64</v>
       </c>
-      <c r="B37" s="12" t="s">
+      <c r="B37" s="3" t="s">
         <v>154</v>
       </c>
       <c r="C37" s="3"/>
     </row>
     <row r="38" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B38" s="12"/>
       <c r="C38" s="3" t="s">
         <v>20</v>
       </c>
@@ -1936,7 +2089,6 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B39" s="12"/>
       <c r="C39" s="3" t="s">
         <v>42</v>
       </c>
@@ -1949,7 +2101,6 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B40" s="12"/>
       <c r="C40" s="3" t="s">
         <v>64</v>
       </c>
@@ -1961,23 +2112,20 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B41" s="12"/>
       <c r="C41" s="3"/>
       <c r="F41" s="5"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B42" s="12"/>
       <c r="C42" s="3"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B43" s="12"/>
       <c r="C43" s="3"/>
     </row>
     <row r="44" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A44" s="14" t="s">
+      <c r="A44" s="12" t="s">
         <v>55</v>
       </c>
-      <c r="B44" s="12" t="s">
+      <c r="B44" s="3" t="s">
         <v>162</v>
       </c>
       <c r="C44" s="3"/>
@@ -1985,7 +2133,6 @@
       <c r="F44" s="2"/>
     </row>
     <row r="45" spans="1:6" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B45" s="12"/>
       <c r="C45" s="3" t="s">
         <v>55</v>
       </c>
@@ -1997,7 +2144,6 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
-      <c r="B46" s="12"/>
       <c r="C46" s="3" t="s">
         <v>66</v>
       </c>
@@ -2009,7 +2155,6 @@
       </c>
     </row>
     <row r="47" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
-      <c r="B47" s="12"/>
       <c r="C47" s="3" t="s">
         <v>31</v>
       </c>
@@ -2024,10 +2169,10 @@
       </c>
     </row>
     <row r="48" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="15" t="s">
+      <c r="A48" s="13" t="s">
         <v>129</v>
       </c>
-      <c r="B48" s="12" t="s">
+      <c r="B48" s="3" t="s">
         <v>163</v>
       </c>
       <c r="C48" s="3"/>
@@ -2035,7 +2180,6 @@
       <c r="F48" s="2"/>
     </row>
     <row r="49" spans="1:6" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B49" s="12"/>
       <c r="C49" s="3" t="s">
         <v>56</v>
       </c>
@@ -2047,7 +2191,6 @@
       </c>
     </row>
     <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B50" s="12"/>
       <c r="C50" s="3" t="s">
         <v>78</v>
       </c>
@@ -2059,7 +2202,6 @@
       </c>
     </row>
     <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B51" s="12"/>
       <c r="C51" s="3" t="s">
         <v>78</v>
       </c>
@@ -2071,7 +2213,6 @@
       </c>
     </row>
     <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B52" s="12"/>
       <c r="C52" s="3" t="s">
         <v>65</v>
       </c>
@@ -2083,7 +2224,6 @@
       </c>
     </row>
     <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B53" s="12"/>
       <c r="C53" s="3" t="s">
         <v>75</v>
       </c>
@@ -2095,17 +2235,16 @@
       </c>
     </row>
     <row r="54" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="15" t="s">
+      <c r="A54" s="13" t="s">
         <v>128</v>
       </c>
-      <c r="B54" s="12" t="s">
+      <c r="B54" s="3" t="s">
         <v>162</v>
       </c>
       <c r="C54" s="3"/>
       <c r="F54" s="5"/>
     </row>
     <row r="55" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B55" s="12"/>
       <c r="C55" s="3" t="s">
         <v>57</v>
       </c>
@@ -2117,7 +2256,6 @@
       </c>
     </row>
     <row r="56" spans="1:6" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B56" s="12"/>
       <c r="C56" s="3" t="s">
         <v>61</v>
       </c>
@@ -2129,7 +2267,6 @@
       </c>
     </row>
     <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B57" s="12"/>
       <c r="C57" s="3" t="s">
         <v>8</v>
       </c>
@@ -2145,13 +2282,12 @@
       <c r="A58" s="8" t="s">
         <v>130</v>
       </c>
-      <c r="B58" s="12" t="s">
+      <c r="B58" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C58" s="3"/>
     </row>
     <row r="59" spans="1:6" ht="35.25" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B59" s="12"/>
       <c r="C59" s="3" t="s">
         <v>36</v>
       </c>
@@ -2165,21 +2301,17 @@
         <v>88</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B60" s="12"/>
-    </row>
     <row r="61" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A61" s="15" t="s">
+      <c r="A61" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B61" s="12" t="s">
+      <c r="B61" s="3" t="s">
         <v>156</v>
       </c>
       <c r="C61" s="3"/>
       <c r="F61" s="5"/>
     </row>
     <row r="62" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B62" s="12"/>
       <c r="C62" s="3" t="s">
         <v>40</v>
       </c>
@@ -2192,7 +2324,6 @@
       </c>
     </row>
     <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B63" s="12"/>
       <c r="C63" s="3" t="s">
         <v>63</v>
       </c>
@@ -2204,7 +2335,6 @@
       </c>
     </row>
     <row r="64" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B64" s="12"/>
       <c r="C64" s="3" t="s">
         <v>26</v>
       </c>
@@ -2217,10 +2347,10 @@
       </c>
     </row>
     <row r="65" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="15" t="s">
+      <c r="A65" s="13" t="s">
         <v>133</v>
       </c>
-      <c r="B65" s="12" t="s">
+      <c r="B65" s="3" t="s">
         <v>157</v>
       </c>
       <c r="C65" s="3"/>
@@ -2228,7 +2358,6 @@
       <c r="F65" s="2"/>
     </row>
     <row r="66" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B66" s="12"/>
       <c r="C66" s="3" t="s">
         <v>44</v>
       </c>
@@ -2241,7 +2370,6 @@
       </c>
     </row>
     <row r="67" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B67" s="12"/>
       <c r="C67" s="3" t="s">
         <v>46</v>
       </c>
@@ -2253,32 +2381,29 @@
       </c>
     </row>
     <row r="68" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
-      <c r="B68" s="12"/>
       <c r="C68" s="3"/>
       <c r="F68" s="2"/>
     </row>
     <row r="69" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A69" s="15" t="s">
+      <c r="A69" s="13" t="s">
         <v>164</v>
       </c>
-      <c r="B69" s="12" t="s">
+      <c r="B69" s="3" t="s">
         <v>165</v>
       </c>
       <c r="C69" s="3"/>
     </row>
     <row r="70" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="B70" s="12"/>
       <c r="C70" s="3"/>
     </row>
     <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="9" t="s">
         <v>132</v>
       </c>
-      <c r="B71" s="12"/>
       <c r="C71" s="3"/>
     </row>
     <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B72" s="12" t="s">
+      <c r="B72" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C72" s="3" t="s">
@@ -2292,7 +2417,7 @@
       </c>
     </row>
     <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B73" s="12" t="s">
+      <c r="B73" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C73" s="3" t="s">
@@ -2306,10 +2431,10 @@
       </c>
     </row>
     <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B74" s="12" t="s">
+      <c r="B74" s="3" t="s">
         <v>158</v>
       </c>
-      <c r="C74" s="16" t="s">
+      <c r="C74" s="14" t="s">
         <v>72</v>
       </c>
       <c r="D74" s="3" t="s">
@@ -2320,10 +2445,10 @@
       </c>
     </row>
     <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B75" s="12" t="s">
+      <c r="B75" s="3" t="s">
         <v>160</v>
       </c>
-      <c r="C75" s="16" t="s">
+      <c r="C75" s="14" t="s">
         <v>74</v>
       </c>
       <c r="D75" s="3" t="s">
@@ -2335,10 +2460,10 @@
     </row>
     <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A76"/>
-      <c r="B76" s="12" t="s">
+      <c r="B76" s="3" t="s">
         <v>161</v>
       </c>
-      <c r="C76" s="16" t="s">
+      <c r="C76" s="14" t="s">
         <v>34</v>
       </c>
       <c r="D76" s="3" t="s">
@@ -2350,7 +2475,7 @@
       </c>
     </row>
     <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B77" s="12" t="s">
+      <c r="B77" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C77" s="3" t="s">
@@ -2365,10 +2490,10 @@
     </row>
     <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
       <c r="A78"/>
-      <c r="B78" s="12" t="s">
+      <c r="B78" s="3" t="s">
         <v>159</v>
       </c>
-      <c r="C78" s="16" t="s">
+      <c r="C78" s="14" t="s">
         <v>76</v>
       </c>
       <c r="D78" s="3" t="s">
@@ -2379,7 +2504,7 @@
       </c>
     </row>
     <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B79" s="12" t="s">
+      <c r="B79" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C79" s="3" t="s">
@@ -2393,7 +2518,7 @@
       </c>
     </row>
     <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B80" s="12" t="s">
+      <c r="B80" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C80" s="3" t="s">
@@ -2407,7 +2532,7 @@
       </c>
     </row>
     <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
-      <c r="B81" s="12" t="s">
+      <c r="B81" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C81" s="3" t="s">
@@ -2421,7 +2546,7 @@
       </c>
     </row>
     <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
-      <c r="B82" s="12" t="s">
+      <c r="B82" s="3" t="s">
         <v>155</v>
       </c>
       <c r="C82" s="3" t="s">
@@ -2435,7 +2560,6 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B83" s="12"/>
       <c r="C83" s="3"/>
     </row>
     <row r="84" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
@@ -2507,73 +2631,40 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B88" s="12"/>
       <c r="C88" s="3"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B89" s="12"/>
       <c r="C89" s="3"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B90" s="12"/>
       <c r="C90" s="3"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B91" s="12"/>
       <c r="C91" s="3"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B92" s="12"/>
       <c r="C92" s="3"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B93" s="12"/>
       <c r="C93" s="3"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B94" s="12"/>
       <c r="C94" s="3"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B95" s="12"/>
       <c r="C95" s="3"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.25">
-      <c r="B96" s="12"/>
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B97" s="12"/>
+    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B98" s="12"/>
+    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B99" s="12"/>
+    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
       <c r="C99" s="3"/>
-    </row>
-    <row r="100" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B100" s="12"/>
-    </row>
-    <row r="101" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B101" s="12"/>
-    </row>
-    <row r="102" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B102" s="12"/>
-    </row>
-    <row r="103" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B103" s="12"/>
-    </row>
-    <row r="104" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B104" s="12"/>
-    </row>
-    <row r="105" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B105" s="12"/>
-    </row>
-    <row r="106" spans="2:3" x14ac:dyDescent="0.25">
-      <c r="B106" s="12"/>
     </row>
   </sheetData>
   <autoFilter ref="F1:F128" xr:uid="{0EE97473-BB80-432A-9BAA-EAC31F0F8EE4}"/>
@@ -2585,603 +2676,603 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45558578-E863-4F34-A55F-1F97248AC422}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="12" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="12" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="12" customWidth="1"/>
-    <col min="4" max="4" width="74.85546875" style="12" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="12"/>
+    <col min="1" max="1" width="25.28515625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.42578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.7109375" style="3" customWidth="1"/>
+    <col min="4" max="4" width="74.85546875" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A1" s="18" t="s">
+      <c r="A1" s="4" t="s">
         <v>293</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="D1" s="3" t="s">
         <v>294</v>
       </c>
     </row>
     <row r="2" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>168</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="16" t="s">
         <v>169</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="16" t="s">
         <v>170</v>
       </c>
-      <c r="D2" s="19" t="s">
+      <c r="D2" s="16" t="s">
         <v>171</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="17" t="s">
+      <c r="A3" s="15" t="s">
         <v>172</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="3" t="s">
         <v>173</v>
       </c>
-      <c r="D3" s="12" t="s">
+      <c r="D3" s="3" t="s">
         <v>174</v>
       </c>
     </row>
     <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B4" s="17" t="s">
+      <c r="B4" s="15" t="s">
         <v>298</v>
       </c>
-      <c r="C4" s="12" t="s">
+      <c r="C4" s="3" t="s">
         <v>175</v>
       </c>
-      <c r="D4" s="12" t="s">
+      <c r="D4" s="3" t="s">
         <v>176</v>
       </c>
     </row>
     <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B5" s="17" t="s">
+      <c r="B5" s="15" t="s">
         <v>299</v>
       </c>
-      <c r="C5" s="12" t="s">
+      <c r="C5" s="3" t="s">
         <v>177</v>
       </c>
-      <c r="D5" s="12" t="s">
+      <c r="D5" s="3" t="s">
         <v>178</v>
       </c>
     </row>
     <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B6" s="17" t="s">
+      <c r="B6" s="15" t="s">
         <v>300</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="3" t="s">
         <v>179</v>
       </c>
-      <c r="D6" s="12" t="s">
+      <c r="D6" s="3" t="s">
         <v>180</v>
       </c>
     </row>
     <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="15" t="s">
         <v>301</v>
       </c>
-      <c r="C7" s="12" t="s">
+      <c r="C7" s="3" t="s">
         <v>181</v>
       </c>
-      <c r="D7" s="12" t="s">
+      <c r="D7" s="3" t="s">
         <v>182</v>
       </c>
     </row>
     <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B8" s="17" t="s">
+      <c r="B8" s="15" t="s">
         <v>302</v>
       </c>
-      <c r="C8" s="12" t="s">
+      <c r="C8" s="3" t="s">
         <v>183</v>
       </c>
-      <c r="D8" s="12" t="s">
+      <c r="D8" s="3" t="s">
         <v>184</v>
       </c>
     </row>
     <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="15" t="s">
         <v>303</v>
       </c>
-      <c r="C9" s="12" t="s">
+      <c r="C9" s="3" t="s">
         <v>185</v>
       </c>
-      <c r="D9" s="12" t="s">
+      <c r="D9" s="3" t="s">
         <v>186</v>
       </c>
     </row>
     <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B10" s="17" t="s">
+      <c r="B10" s="15" t="s">
         <v>304</v>
       </c>
-      <c r="C10" s="12" t="s">
+      <c r="C10" s="3" t="s">
         <v>187</v>
       </c>
-      <c r="D10" s="12" t="s">
+      <c r="D10" s="3" t="s">
         <v>188</v>
       </c>
     </row>
     <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
-      <c r="A11" s="17" t="s">
+      <c r="A11" s="15" t="s">
         <v>189</v>
       </c>
-      <c r="C11" s="12" t="s">
+      <c r="C11" s="3" t="s">
         <v>190</v>
       </c>
-      <c r="D11" s="12" t="s">
+      <c r="D11" s="3" t="s">
         <v>191</v>
       </c>
     </row>
     <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A12" s="17" t="s">
+      <c r="A12" s="15" t="s">
         <v>192</v>
       </c>
-      <c r="C12" s="12" t="s">
+      <c r="C12" s="3" t="s">
         <v>193</v>
       </c>
-      <c r="D12" s="12" t="s">
+      <c r="D12" s="3" t="s">
         <v>194</v>
       </c>
     </row>
     <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A13" s="17" t="s">
+      <c r="A13" s="15" t="s">
         <v>195</v>
       </c>
-      <c r="C13" s="12" t="s">
+      <c r="C13" s="3" t="s">
         <v>196</v>
       </c>
-      <c r="D13" s="12" t="s">
+      <c r="D13" s="3" t="s">
         <v>197</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="17" t="s">
+      <c r="A14" s="15" t="s">
         <v>198</v>
       </c>
-      <c r="C14" s="12" t="s">
+      <c r="C14" s="3" t="s">
         <v>199</v>
       </c>
-      <c r="D14" s="12" t="s">
+      <c r="D14" s="3" t="s">
         <v>200</v>
       </c>
     </row>
     <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A15" s="17" t="s">
+      <c r="A15" s="15" t="s">
         <v>201</v>
       </c>
-      <c r="C15" s="12" t="s">
+      <c r="C15" s="3" t="s">
         <v>202</v>
       </c>
-      <c r="D15" s="12" t="s">
+      <c r="D15" s="3" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A16" s="17" t="s">
+      <c r="A16" s="15" t="s">
         <v>204</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="3" t="s">
         <v>205</v>
       </c>
-      <c r="D16" s="12" t="s">
+      <c r="D16" s="3" t="s">
         <v>206</v>
       </c>
     </row>
     <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B17" s="17" t="s">
+      <c r="B17" s="15" t="s">
         <v>305</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="3" t="s">
         <v>207</v>
       </c>
-      <c r="D17" s="12" t="s">
+      <c r="D17" s="3" t="s">
         <v>208</v>
       </c>
     </row>
     <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B18" s="17" t="s">
+      <c r="B18" s="15" t="s">
         <v>306</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="3" t="s">
         <v>209</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="3" t="s">
         <v>210</v>
       </c>
     </row>
     <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B19" s="17" t="s">
+      <c r="B19" s="15" t="s">
         <v>307</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="3" t="s">
         <v>211</v>
       </c>
-      <c r="D19" s="12" t="s">
+      <c r="D19" s="3" t="s">
         <v>212</v>
       </c>
     </row>
     <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B20" s="17" t="s">
+      <c r="B20" s="15" t="s">
         <v>308</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="D20" s="12" t="s">
+      <c r="D20" s="3" t="s">
         <v>214</v>
       </c>
     </row>
     <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A21" s="17" t="s">
+      <c r="A21" s="15" t="s">
         <v>215</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="3" t="s">
         <v>216</v>
       </c>
-      <c r="D21" s="12" t="s">
+      <c r="D21" s="3" t="s">
         <v>217</v>
       </c>
     </row>
     <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A22" s="17" t="s">
+      <c r="A22" s="15" t="s">
         <v>218</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="3" t="s">
         <v>219</v>
       </c>
-      <c r="D22" s="12" t="s">
+      <c r="D22" s="3" t="s">
         <v>220</v>
       </c>
     </row>
     <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A23" s="17" t="s">
+      <c r="A23" s="15" t="s">
         <v>221</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="3" t="s">
         <v>222</v>
       </c>
-      <c r="D23" s="12" t="s">
+      <c r="D23" s="3" t="s">
         <v>223</v>
       </c>
     </row>
     <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A24" s="17" t="s">
+      <c r="A24" s="15" t="s">
         <v>224</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="3" t="s">
         <v>225</v>
       </c>
-      <c r="D24" s="12" t="s">
+      <c r="D24" s="3" t="s">
         <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+      <c r="A25" s="15" t="s">
         <v>227</v>
       </c>
-      <c r="C25" s="12" t="s">
+      <c r="C25" s="3" t="s">
         <v>228</v>
       </c>
-      <c r="D25" s="12" t="s">
+      <c r="D25" s="3" t="s">
         <v>229</v>
       </c>
     </row>
     <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="17" t="s">
+      <c r="A26" s="15" t="s">
         <v>230</v>
       </c>
-      <c r="C26" s="12" t="s">
+      <c r="C26" s="3" t="s">
         <v>230</v>
       </c>
-      <c r="D26" s="12" t="s">
+      <c r="D26" s="3" t="s">
         <v>231</v>
       </c>
     </row>
     <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A27" s="17" t="s">
+      <c r="A27" s="15" t="s">
         <v>232</v>
       </c>
-      <c r="C27" s="12" t="s">
+      <c r="C27" s="3" t="s">
         <v>232</v>
       </c>
-      <c r="D27" s="12" t="s">
+      <c r="D27" s="3" t="s">
         <v>233</v>
       </c>
     </row>
     <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A28" s="17" t="s">
+      <c r="A28" s="15" t="s">
         <v>234</v>
       </c>
-      <c r="C28" s="12" t="s">
+      <c r="C28" s="3" t="s">
         <v>235</v>
       </c>
-      <c r="D28" s="12" t="s">
+      <c r="D28" s="3" t="s">
         <v>236</v>
       </c>
     </row>
     <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A29" s="17" t="s">
+      <c r="A29" s="15" t="s">
         <v>237</v>
       </c>
-      <c r="C29" s="12" t="s">
+      <c r="C29" s="3" t="s">
         <v>237</v>
       </c>
-      <c r="D29" s="12" t="s">
+      <c r="D29" s="3" t="s">
         <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="17" t="s">
+      <c r="A30" s="15" t="s">
         <v>239</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="3" t="s">
         <v>240</v>
       </c>
-      <c r="D30" s="12" t="s">
+      <c r="D30" s="3" t="s">
         <v>241</v>
       </c>
     </row>
     <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A31" s="17" t="s">
+      <c r="A31" s="15" t="s">
         <v>242</v>
       </c>
-      <c r="C31" s="12" t="s">
+      <c r="C31" s="3" t="s">
         <v>242</v>
       </c>
-      <c r="D31" s="12" t="s">
+      <c r="D31" s="3" t="s">
         <v>243</v>
       </c>
     </row>
     <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A32" s="17" t="s">
+      <c r="A32" s="15" t="s">
         <v>244</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="3" t="s">
         <v>245</v>
       </c>
-      <c r="D32" s="12" t="s">
+      <c r="D32" s="3" t="s">
         <v>246</v>
       </c>
     </row>
     <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
+      <c r="A33" s="15" t="s">
         <v>247</v>
       </c>
-      <c r="C33" s="12" t="s">
+      <c r="C33" s="3" t="s">
         <v>248</v>
       </c>
-      <c r="D33" s="12" t="s">
+      <c r="D33" s="3" t="s">
         <v>249</v>
       </c>
     </row>
     <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="A34" s="17" t="s">
+      <c r="A34" s="15" t="s">
         <v>250</v>
       </c>
-      <c r="C34" s="12" t="s">
+      <c r="C34" s="3" t="s">
         <v>250</v>
       </c>
-      <c r="D34" s="12" t="s">
+      <c r="D34" s="3" t="s">
         <v>251</v>
       </c>
     </row>
     <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A35" s="17" t="s">
+      <c r="A35" s="15" t="s">
         <v>252</v>
       </c>
-      <c r="C35" s="12" t="s">
+      <c r="C35" s="3" t="s">
         <v>253</v>
       </c>
-      <c r="D35" s="12" t="s">
+      <c r="D35" s="3" t="s">
         <v>254</v>
       </c>
     </row>
     <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A36" s="17" t="s">
+      <c r="A36" s="15" t="s">
         <v>255</v>
       </c>
-      <c r="C36" s="12" t="s">
+      <c r="C36" s="3" t="s">
         <v>256</v>
       </c>
-      <c r="D36" s="12" t="s">
+      <c r="D36" s="3" t="s">
         <v>257</v>
       </c>
     </row>
     <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="B37" s="17" t="s">
+      <c r="B37" s="15" t="s">
         <v>295</v>
       </c>
-      <c r="C37" s="12" t="s">
+      <c r="C37" s="3" t="s">
         <v>258</v>
       </c>
-      <c r="D37" s="12" t="s">
+      <c r="D37" s="3" t="s">
         <v>259</v>
       </c>
     </row>
     <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
-      <c r="B38" s="17" t="s">
+      <c r="B38" s="15" t="s">
         <v>296</v>
       </c>
-      <c r="C38" s="12" t="s">
+      <c r="C38" s="3" t="s">
         <v>260</v>
       </c>
-      <c r="D38" s="12" t="s">
+      <c r="D38" s="3" t="s">
         <v>261</v>
       </c>
     </row>
     <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B39" s="17" t="s">
+      <c r="B39" s="15" t="s">
         <v>297</v>
       </c>
-      <c r="C39" s="12" t="s">
+      <c r="C39" s="3" t="s">
         <v>262</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="3" t="s">
         <v>263</v>
       </c>
     </row>
     <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A40" s="17" t="s">
+      <c r="A40" s="15" t="s">
         <v>264</v>
       </c>
-      <c r="C40" s="12" t="s">
+      <c r="C40" s="3" t="s">
         <v>264</v>
       </c>
-      <c r="D40" s="12" t="s">
+      <c r="D40" s="3" t="s">
         <v>265</v>
       </c>
     </row>
     <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A41" s="17" t="s">
+      <c r="A41" s="15" t="s">
         <v>59</v>
       </c>
-      <c r="C41" s="12" t="s">
+      <c r="C41" s="3" t="s">
         <v>266</v>
       </c>
-      <c r="D41" s="12" t="s">
+      <c r="D41" s="3" t="s">
         <v>267</v>
       </c>
     </row>
     <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A42" s="17" t="s">
+      <c r="A42" s="15" t="s">
         <v>61</v>
       </c>
-      <c r="C42" s="12" t="s">
+      <c r="C42" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="D42" s="12" t="s">
+      <c r="D42" s="3" t="s">
         <v>268</v>
       </c>
     </row>
     <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A43" s="17" t="s">
+      <c r="A43" s="15" t="s">
         <v>62</v>
       </c>
-      <c r="C43" s="12" t="s">
+      <c r="C43" s="3" t="s">
         <v>269</v>
       </c>
-      <c r="D43" s="12" t="s">
+      <c r="D43" s="3" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A44" s="17" t="s">
+      <c r="A44" s="15" t="s">
         <v>271</v>
       </c>
-      <c r="C44" s="12" t="s">
+      <c r="C44" s="3" t="s">
         <v>272</v>
       </c>
-      <c r="D44" s="12" t="s">
+      <c r="D44" s="3" t="s">
         <v>273</v>
       </c>
     </row>
     <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A45" s="17" t="s">
+      <c r="A45" s="15" t="s">
         <v>274</v>
       </c>
-      <c r="C45" s="12" t="s">
+      <c r="C45" s="3" t="s">
         <v>275</v>
       </c>
-      <c r="D45" s="12" t="s">
+      <c r="D45" s="3" t="s">
         <v>276</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A46" s="17" t="s">
+      <c r="A46" s="15" t="s">
         <v>277</v>
       </c>
-      <c r="C46" s="12" t="s">
+      <c r="C46" s="3" t="s">
         <v>278</v>
       </c>
-      <c r="D46" s="12" t="s">
+      <c r="D46" s="3" t="s">
         <v>279</v>
       </c>
     </row>
     <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A47" s="17" t="s">
+      <c r="A47" s="15" t="s">
         <v>78</v>
       </c>
-      <c r="C47" s="12" t="s">
+      <c r="C47" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="D47" s="12" t="s">
+      <c r="D47" s="3" t="s">
         <v>280</v>
       </c>
     </row>
     <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
-      <c r="A48" s="17" t="s">
+      <c r="A48" s="15" t="s">
         <v>281</v>
       </c>
-      <c r="C48" s="12" t="s">
+      <c r="C48" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="D48" s="12" t="s">
+      <c r="D48" s="3" t="s">
         <v>282</v>
       </c>
     </row>
     <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A49" s="17" t="s">
+      <c r="A49" s="15" t="s">
         <v>283</v>
       </c>
-      <c r="C49" s="12" t="s">
+      <c r="C49" s="3" t="s">
         <v>283</v>
       </c>
-      <c r="D49" s="12" t="s">
+      <c r="D49" s="3" t="s">
         <v>284</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A50" s="17" t="s">
+      <c r="A50" s="15" t="s">
         <v>285</v>
       </c>
-      <c r="C50" s="12" t="s">
+      <c r="C50" s="3" t="s">
         <v>286</v>
       </c>
-      <c r="D50" s="12" t="s">
+      <c r="D50" s="3" t="s">
         <v>287</v>
       </c>
     </row>
     <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A51" s="17" t="s">
+      <c r="A51" s="15" t="s">
         <v>80</v>
       </c>
-      <c r="C51" s="12" t="s">
+      <c r="C51" s="3" t="s">
         <v>80</v>
       </c>
-      <c r="D51" s="12" t="s">
+      <c r="D51" s="3" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A52" s="17" t="s">
+      <c r="A52" s="15" t="s">
         <v>289</v>
       </c>
-      <c r="C52" s="12" t="s">
+      <c r="C52" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="D52" s="12" t="s">
+      <c r="D52" s="3" t="s">
         <v>291</v>
       </c>
     </row>
     <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A53" s="17" t="s">
+      <c r="A53" s="15" t="s">
         <v>67</v>
       </c>
-      <c r="C53" s="12" t="s">
+      <c r="C53" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="D53" s="12" t="s">
+      <c r="D53" s="3" t="s">
         <v>292</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update role vocabulary compilation
</commit_message>
<xml_diff>
--- a/notes/vocabulary/RoleVocabulary.xlsx
+++ b/notes/vocabulary/RoleVocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GithubC\iSamples\metadata\notes\vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B627D58-173D-4019-A5C2-FA00A615D56B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEA1FF3-F25E-4A70-BA37-FAD91AB798A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="24060" windowHeight="15270" activeTab="2" xr2:uid="{6D09EB57-77EB-4B90-8113-743A5CC7E14E}"/>
+    <workbookView xWindow="60" yWindow="540" windowWidth="13010" windowHeight="8500" xr2:uid="{6D09EB57-77EB-4B90-8113-743A5CC7E14E}"/>
   </bookViews>
   <sheets>
     <sheet name="synthesis" sheetId="3" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="319">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="451" uniqueCount="338">
   <si>
     <t>Entry</t>
   </si>
@@ -969,15 +969,9 @@
     <t>DataProcessing. DataValidation</t>
   </si>
   <si>
-    <t>role</t>
-  </si>
-  <si>
     <t>scope note</t>
   </si>
   <si>
-    <t>Who is responsible for providing access to  the sample (or part of it) for research</t>
-  </si>
-  <si>
     <t>ISO19115-1, DataCite4.4</t>
   </si>
   <si>
@@ -987,9 +981,6 @@
     <t>DataCredit, casRAI,ISO19115-1, DataCite4.4</t>
   </si>
   <si>
-    <t>Role related to Initiative or Curation-- Leader of project that supported sample collection or curation activities</t>
-  </si>
-  <si>
     <t>Role related to Initiative or Curation-- Manager of project that supported sample collection activities; might not be necessary</t>
   </si>
   <si>
@@ -997,6 +988,72 @@
   </si>
   <si>
     <t>Person on the membership list of a designated project/project team</t>
+  </si>
+  <si>
+    <t>Who is responsible for providing access to  the sample (or part of it) for research. Typically an organization.</t>
+  </si>
+  <si>
+    <t>Who collected the sample. Generally should be a person or project.</t>
+  </si>
+  <si>
+    <t>who is responsible for sample preservation and maintenance. Person or Organization.</t>
+  </si>
+  <si>
+    <t>Who funded or otherwise provided material support for an activity. In the samples model, the domain is initiative. Typyically an organization.</t>
+  </si>
+  <si>
+    <t>Role related to Initiative or Curation-- Leader of project that supported sample collection or curation activities. Should be a Person</t>
+  </si>
+  <si>
+    <t>sample owner</t>
+  </si>
+  <si>
+    <t>metadata publisher</t>
+  </si>
+  <si>
+    <t>curation</t>
+  </si>
+  <si>
+    <t>label</t>
+  </si>
+  <si>
+    <t>point of contact</t>
+  </si>
+  <si>
+    <t>other contributor</t>
+  </si>
+  <si>
+    <t>collector</t>
+  </si>
+  <si>
+    <t>curator</t>
+  </si>
+  <si>
+    <t>project leader</t>
+  </si>
+  <si>
+    <t>manager</t>
+  </si>
+  <si>
+    <t>team member</t>
+  </si>
+  <si>
+    <t>rights holder</t>
+  </si>
+  <si>
+    <t>registrant</t>
+  </si>
+  <si>
+    <t>who owns or has legal authority for sample management (? Should this be sample owner? )</t>
+  </si>
+  <si>
+    <t>Agent who is responsible for making metadata public. Not necessarily the same as the agent reponsible for metadata content.</t>
+  </si>
+  <si>
+    <t>identified by</t>
+  </si>
+  <si>
+    <t>person who assigned sample to a biological taxon or other category</t>
   </si>
 </sst>
 </file>
@@ -1114,7 +1171,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
@@ -1162,6 +1219,9 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1480,10 +1540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8140B6-11ED-4C30-ABC1-8C066247C7B6}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A12" sqref="A12:B12"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1494,42 +1554,42 @@
     <col min="4" max="16384" width="9.140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
+        <v>324</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>309</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>310</v>
       </c>
       <c r="C1" s="3" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A2" s="3" t="s">
-        <v>51</v>
+    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="17" t="s">
+        <v>15</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>311</v>
+        <v>316</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A3" s="3" t="s">
-        <v>166</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
+        <v>325</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>148</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" s="3" t="s">
-        <v>127</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="17" t="s">
+        <v>326</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -1538,94 +1598,122 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A5" s="3" t="s">
-        <v>134</v>
+    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A5" s="17" t="s">
+        <v>327</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>151</v>
+        <v>317</v>
       </c>
       <c r="C5" s="3" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+      <c r="A6" s="17" t="s">
+        <v>328</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>312</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A7" s="17" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="C7" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A8" s="17" t="s">
+        <v>329</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A9" s="17" t="s">
+        <v>330</v>
+      </c>
+      <c r="B9" s="3" t="s">
         <v>313</v>
       </c>
-    </row>
-    <row r="6" spans="1:3" ht="45" x14ac:dyDescent="0.25">
-      <c r="A6" s="3" t="s">
-        <v>135</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>152</v>
-      </c>
-      <c r="C6" s="3" t="s">
+      <c r="C9" s="3" t="s">
         <v>314</v>
       </c>
     </row>
-    <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A7" s="3" t="s">
-        <v>64</v>
-      </c>
-      <c r="B7" s="3" t="s">
-        <v>154</v>
-      </c>
-      <c r="C7" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A8" s="3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B8" s="3" t="s">
+    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A10" s="17" t="s">
+        <v>331</v>
+      </c>
+      <c r="B10" s="3" t="s">
         <v>315</v>
       </c>
-      <c r="C8" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A9" s="3" t="s">
-        <v>129</v>
-      </c>
-      <c r="B9" s="3" t="s">
-        <v>316</v>
-      </c>
-      <c r="C9" s="3" t="s">
-        <v>317</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A10" s="3" t="s">
-        <v>128</v>
-      </c>
-      <c r="B10" s="3" t="s">
-        <v>318</v>
-      </c>
       <c r="C10" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A11" s="3" t="s">
-        <v>63</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A11" s="17" t="s">
+        <v>332</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>156</v>
+        <v>334</v>
       </c>
       <c r="C11" s="3" t="s">
-        <v>312</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" s="3" t="s">
-        <v>164</v>
+        <v>310</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" s="17" t="s">
+        <v>333</v>
       </c>
       <c r="B12" s="3" t="s">
         <v>165</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A14" s="17" t="s">
+        <v>321</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A15" s="17" t="s">
+        <v>322</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>335</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A16" s="3" t="s">
+        <v>336</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>337</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -2680,7 +2768,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{45558578-E863-4F34-A55F-1F97248AC422}">
   <dimension ref="A1:D53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
add draft for OpenContext incremental metadata
the ProjectMetadataWorkflow.docx lays out metadata at project, sampling event, and individual sample level. Yaml is a json file converted to yaml so I could add comments.
</commit_message>
<xml_diff>
--- a/notes/vocabulary/RoleVocabulary.xlsx
+++ b/notes/vocabulary/RoleVocabulary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GithubC\iSamples\metadata\notes\vocabulary\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2FEA1FF3-F25E-4A70-BA37-FAD91AB798A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8B3BD0F5-9247-4ACF-AD7F-B7FEA0F5014A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="60" yWindow="540" windowWidth="13010" windowHeight="8500" xr2:uid="{6D09EB57-77EB-4B90-8113-743A5CC7E14E}"/>
+    <workbookView xWindow="60" yWindow="540" windowWidth="17630" windowHeight="9490" activeTab="1" xr2:uid="{6D09EB57-77EB-4B90-8113-743A5CC7E14E}"/>
   </bookViews>
   <sheets>
     <sheet name="synthesis" sheetId="3" r:id="rId1"/>
@@ -1542,19 +1542,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8140B6-11ED-4C30-ABC1-8C066247C7B6}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+    <sheetView topLeftCell="A12" workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="22.42578125" style="3" customWidth="1"/>
-    <col min="2" max="2" width="65.7109375" style="3" customWidth="1"/>
-    <col min="3" max="3" width="21.42578125" style="3" customWidth="1"/>
-    <col min="4" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="22.453125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="65.7265625" style="3" customWidth="1"/>
+    <col min="3" max="3" width="21.453125" style="3" customWidth="1"/>
+    <col min="4" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A1" s="3" t="s">
         <v>324</v>
       </c>
@@ -1565,7 +1565,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>15</v>
       </c>
@@ -1576,7 +1576,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="17" t="s">
         <v>325</v>
       </c>
@@ -1587,7 +1587,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="17" t="s">
         <v>326</v>
       </c>
@@ -1598,7 +1598,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>327</v>
       </c>
@@ -1609,7 +1609,7 @@
         <v>311</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A6" s="17" t="s">
         <v>328</v>
       </c>
@@ -1620,7 +1620,7 @@
         <v>312</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A7" s="17" t="s">
         <v>42</v>
       </c>
@@ -1631,7 +1631,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A8" s="17" t="s">
         <v>329</v>
       </c>
@@ -1642,7 +1642,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A9" s="17" t="s">
         <v>330</v>
       </c>
@@ -1653,7 +1653,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="17" t="s">
         <v>331</v>
       </c>
@@ -1664,7 +1664,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A11" s="17" t="s">
         <v>332</v>
       </c>
@@ -1675,7 +1675,7 @@
         <v>310</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="17" t="s">
         <v>333</v>
       </c>
@@ -1683,7 +1683,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="17" t="s">
         <v>321</v>
       </c>
@@ -1691,7 +1691,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="17" t="s">
         <v>322</v>
       </c>
@@ -1702,7 +1702,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="3" t="s">
         <v>336</v>
       </c>
@@ -1721,23 +1721,23 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{52C4C688-E06A-402C-B8FF-1231BDDB6C39}">
   <dimension ref="A1:F99"/>
   <sheetViews>
-    <sheetView topLeftCell="A72" workbookViewId="0">
-      <selection activeCell="A69" sqref="A69:B69"/>
+    <sheetView tabSelected="1" topLeftCell="A85" workbookViewId="0">
+      <selection activeCell="F18" sqref="F18:F21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="23" style="4" customWidth="1"/>
-    <col min="2" max="2" width="43.5703125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="31.42578125" style="4" customWidth="1"/>
-    <col min="4" max="4" width="54.85546875" style="3" customWidth="1"/>
-    <col min="5" max="5" width="35.7109375" style="4" customWidth="1"/>
-    <col min="6" max="6" width="20.5703125" style="4" customWidth="1"/>
-    <col min="7" max="7" width="26.42578125" style="4" customWidth="1"/>
-    <col min="8" max="16384" width="9.140625" style="4"/>
+    <col min="2" max="2" width="43.54296875" style="3" customWidth="1"/>
+    <col min="3" max="3" width="31.453125" style="4" customWidth="1"/>
+    <col min="4" max="4" width="54.81640625" style="3" customWidth="1"/>
+    <col min="5" max="5" width="35.7265625" style="4" customWidth="1"/>
+    <col min="6" max="6" width="20.54296875" style="4" customWidth="1"/>
+    <col min="7" max="7" width="26.453125" style="4" customWidth="1"/>
+    <col min="8" max="16384" width="9.1796875" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" s="8" t="s">
         <v>90</v>
       </c>
@@ -1757,7 +1757,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="46.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="30" thickTop="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="12" t="s">
         <v>166</v>
       </c>
@@ -1769,7 +1769,7 @@
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
     </row>
-    <row r="3" spans="1:6" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="73" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C3" s="4" t="s">
         <v>137</v>
       </c>
@@ -1780,7 +1780,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A4" s="2"/>
       <c r="C4" s="3" t="s">
         <v>28</v>
@@ -1795,7 +1795,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="35.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:6" ht="35.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A5" s="7" t="s">
         <v>144</v>
       </c>
@@ -1808,7 +1808,7 @@
       </c>
       <c r="F5" s="2"/>
     </row>
-    <row r="6" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C6" s="3" t="s">
         <v>3</v>
       </c>
@@ -1820,7 +1820,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C7" s="3" t="s">
         <v>24</v>
       </c>
@@ -1831,7 +1831,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C8" s="3" t="s">
         <v>81</v>
       </c>
@@ -1842,7 +1842,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" ht="18" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A9" s="9" t="s">
         <v>167</v>
       </c>
@@ -1860,11 +1860,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C10" s="3"/>
       <c r="F10" s="5"/>
     </row>
-    <row r="11" spans="1:6" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A11" s="10" t="s">
         <v>54</v>
       </c>
@@ -1881,7 +1881,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A12" s="8" t="s">
         <v>52</v>
       </c>
@@ -1889,7 +1889,7 @@
         <v>149</v>
       </c>
     </row>
-    <row r="13" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C13" s="3" t="s">
         <v>18</v>
       </c>
@@ -1901,7 +1901,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="14" spans="1:6" ht="75" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C14" s="3" t="s">
         <v>52</v>
       </c>
@@ -1912,7 +1912,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="15" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C15" s="3" t="s">
         <v>82</v>
       </c>
@@ -1923,7 +1923,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="16" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A16" s="8" t="s">
         <v>126</v>
       </c>
@@ -1933,7 +1933,7 @@
       <c r="C16" s="3"/>
       <c r="F16" s="2"/>
     </row>
-    <row r="17" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C17" s="3" t="s">
         <v>77</v>
       </c>
@@ -1944,7 +1944,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="18" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C18" s="3" t="s">
         <v>77</v>
       </c>
@@ -1955,7 +1955,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="19" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="13" t="s">
         <v>127</v>
       </c>
@@ -1965,7 +1965,7 @@
       <c r="C19" s="3"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C20" s="3" t="s">
         <v>10</v>
       </c>
@@ -1977,7 +1977,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="21" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C21" s="3" t="s">
         <v>60</v>
       </c>
@@ -1988,7 +1988,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="22" spans="1:6" ht="150" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:6" ht="130.5" x14ac:dyDescent="0.35">
       <c r="C22" s="3" t="s">
         <v>67</v>
       </c>
@@ -1999,7 +1999,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="23" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A23" s="13" t="s">
         <v>134</v>
       </c>
@@ -2009,7 +2009,7 @@
       <c r="C23" s="3"/>
       <c r="F23" s="2"/>
     </row>
-    <row r="24" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C24" s="3" t="s">
         <v>84</v>
       </c>
@@ -2020,7 +2020,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:6" ht="72.5" x14ac:dyDescent="0.35">
       <c r="C25" s="3" t="s">
         <v>48</v>
       </c>
@@ -2031,7 +2031,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="26" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="13" t="s">
         <v>135</v>
       </c>
@@ -2040,7 +2040,7 @@
       </c>
       <c r="C26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C27" s="3" t="s">
         <v>85</v>
       </c>
@@ -2051,7 +2051,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="28" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C28" s="3" t="s">
         <v>70</v>
       </c>
@@ -2062,7 +2062,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="29" spans="1:6" ht="240" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:6" ht="217.5" x14ac:dyDescent="0.35">
       <c r="C29" s="3" t="s">
         <v>49</v>
       </c>
@@ -2073,7 +2073,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="30" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="C30" s="3" t="s">
         <v>50</v>
       </c>
@@ -2084,7 +2084,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="31" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C31" s="3" t="s">
         <v>12</v>
       </c>
@@ -2098,7 +2098,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="32" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A32" s="13" t="s">
         <v>51</v>
       </c>
@@ -2109,7 +2109,7 @@
       <c r="E32" s="2"/>
       <c r="F32" s="2"/>
     </row>
-    <row r="33" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C33" s="3" t="s">
         <v>15</v>
       </c>
@@ -2121,7 +2121,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="34" spans="1:6" ht="60" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:6" ht="58" x14ac:dyDescent="0.35">
       <c r="C34" s="3" t="s">
         <v>51</v>
       </c>
@@ -2132,7 +2132,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="35" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C35" s="3" t="s">
         <v>38</v>
       </c>
@@ -2144,7 +2144,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="36" spans="1:6" ht="135" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:6" ht="116" x14ac:dyDescent="0.35">
       <c r="C36" s="3" t="s">
         <v>53</v>
       </c>
@@ -2155,7 +2155,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="37" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A37" s="13" t="s">
         <v>64</v>
       </c>
@@ -2164,7 +2164,7 @@
       </c>
       <c r="C37" s="3"/>
     </row>
-    <row r="38" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C38" s="3" t="s">
         <v>20</v>
       </c>
@@ -2176,7 +2176,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="39" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C39" s="3" t="s">
         <v>42</v>
       </c>
@@ -2188,7 +2188,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="40" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C40" s="3" t="s">
         <v>64</v>
       </c>
@@ -2199,17 +2199,17 @@
         <v>89</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C41" s="3"/>
       <c r="F41" s="5"/>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C42" s="3"/>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C43" s="3"/>
     </row>
-    <row r="44" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A44" s="12" t="s">
         <v>55</v>
       </c>
@@ -2220,7 +2220,7 @@
       <c r="E44" s="2"/>
       <c r="F44" s="2"/>
     </row>
-    <row r="45" spans="1:6" ht="90.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:6" ht="87.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C45" s="3" t="s">
         <v>55</v>
       </c>
@@ -2231,7 +2231,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="46" spans="1:6" ht="90" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:6" ht="87" x14ac:dyDescent="0.35">
       <c r="C46" s="3" t="s">
         <v>66</v>
       </c>
@@ -2242,7 +2242,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="47" spans="1:6" ht="34.5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:6" ht="35" x14ac:dyDescent="0.35">
       <c r="C47" s="3" t="s">
         <v>31</v>
       </c>
@@ -2256,7 +2256,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="48" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:6" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A48" s="13" t="s">
         <v>129</v>
       </c>
@@ -2267,7 +2267,7 @@
       <c r="E48" s="2"/>
       <c r="F48" s="2"/>
     </row>
-    <row r="49" spans="1:6" ht="75.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:6" ht="58.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C49" s="3" t="s">
         <v>56</v>
       </c>
@@ -2278,7 +2278,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="50" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C50" s="3" t="s">
         <v>78</v>
       </c>
@@ -2289,7 +2289,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="51" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C51" s="3" t="s">
         <v>78</v>
       </c>
@@ -2300,7 +2300,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="52" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="C52" s="3" t="s">
         <v>65</v>
       </c>
@@ -2311,7 +2311,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="53" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C53" s="3" t="s">
         <v>75</v>
       </c>
@@ -2322,7 +2322,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="54" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A54" s="13" t="s">
         <v>128</v>
       </c>
@@ -2332,7 +2332,7 @@
       <c r="C54" s="3"/>
       <c r="F54" s="5"/>
     </row>
-    <row r="55" spans="1:6" ht="60.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:6" ht="44" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C55" s="3" t="s">
         <v>57</v>
       </c>
@@ -2343,7 +2343,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="56" spans="1:6" ht="132.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:6" ht="132.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="C56" s="3" t="s">
         <v>61</v>
       </c>
@@ -2354,7 +2354,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="57" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C57" s="3" t="s">
         <v>8</v>
       </c>
@@ -2366,7 +2366,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="58" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A58" s="8" t="s">
         <v>130</v>
       </c>
@@ -2375,7 +2375,7 @@
       </c>
       <c r="C58" s="3"/>
     </row>
-    <row r="59" spans="1:6" ht="35.25" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:6" ht="35.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C59" s="3" t="s">
         <v>36</v>
       </c>
@@ -2389,7 +2389,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="61" spans="1:6" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A61" s="13" t="s">
         <v>63</v>
       </c>
@@ -2399,7 +2399,7 @@
       <c r="C61" s="3"/>
       <c r="F61" s="5"/>
     </row>
-    <row r="62" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:6" ht="18" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C62" s="3" t="s">
         <v>40</v>
       </c>
@@ -2411,7 +2411,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="63" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="C63" s="3" t="s">
         <v>63</v>
       </c>
@@ -2422,7 +2422,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="64" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C64" s="3" t="s">
         <v>26</v>
       </c>
@@ -2434,7 +2434,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:6" ht="29.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A65" s="13" t="s">
         <v>133</v>
       </c>
@@ -2445,7 +2445,7 @@
       <c r="E65" s="2"/>
       <c r="F65" s="2"/>
     </row>
-    <row r="66" spans="1:6" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:6" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C66" s="3" t="s">
         <v>44</v>
       </c>
@@ -2457,7 +2457,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C67" s="3" t="s">
         <v>46</v>
       </c>
@@ -2468,11 +2468,11 @@
         <v>88</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:6" ht="17.5" x14ac:dyDescent="0.35">
       <c r="C68" s="3"/>
       <c r="F68" s="2"/>
     </row>
-    <row r="69" spans="1:6" ht="20.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:6" ht="20" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A69" s="13" t="s">
         <v>164</v>
       </c>
@@ -2481,16 +2481,16 @@
       </c>
       <c r="C69" s="3"/>
     </row>
-    <row r="70" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:6" ht="15" thickTop="1" x14ac:dyDescent="0.35">
       <c r="C70" s="3"/>
     </row>
-    <row r="71" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A71" s="9" t="s">
         <v>132</v>
       </c>
       <c r="C71" s="3"/>
     </row>
-    <row r="72" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B72" s="3" t="s">
         <v>155</v>
       </c>
@@ -2504,7 +2504,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B73" s="3" t="s">
         <v>155</v>
       </c>
@@ -2518,7 +2518,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B74" s="3" t="s">
         <v>158</v>
       </c>
@@ -2532,7 +2532,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="75" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:6" x14ac:dyDescent="0.35">
       <c r="B75" s="3" t="s">
         <v>160</v>
       </c>
@@ -2546,7 +2546,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A76"/>
       <c r="B76" s="3" t="s">
         <v>161</v>
@@ -2562,7 +2562,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B77" s="3" t="s">
         <v>155</v>
       </c>
@@ -2576,7 +2576,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A78"/>
       <c r="B78" s="3" t="s">
         <v>159</v>
@@ -2591,7 +2591,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:6" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B79" s="3" t="s">
         <v>155</v>
       </c>
@@ -2605,7 +2605,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B80" s="3" t="s">
         <v>155</v>
       </c>
@@ -2619,7 +2619,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="81" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B81" s="3" t="s">
         <v>155</v>
       </c>
@@ -2633,7 +2633,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="82" spans="1:6" ht="45" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="B82" s="3" t="s">
         <v>155</v>
       </c>
@@ -2647,10 +2647,10 @@
         <v>68</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C83" s="3"/>
     </row>
-    <row r="84" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:6" ht="58.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A84" s="10" t="s">
         <v>62</v>
       </c>
@@ -2667,7 +2667,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="85" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:6" ht="29" x14ac:dyDescent="0.35">
       <c r="A85" s="4" t="s">
         <v>136</v>
       </c>
@@ -2684,7 +2684,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="86" spans="1:6" ht="120.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:6" ht="102" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A86" s="10" t="s">
         <v>58</v>
       </c>
@@ -2701,7 +2701,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="87" spans="1:6" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:6" ht="73" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A87" s="10" t="s">
         <v>59</v>
       </c>
@@ -2718,40 +2718,40 @@
         <v>89</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C88" s="3"/>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C89" s="3"/>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C90" s="3"/>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C91" s="3"/>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C92" s="3"/>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C93" s="3"/>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C94" s="3"/>
     </row>
-    <row r="95" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C95" s="3"/>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.35">
       <c r="C96" s="3"/>
     </row>
-    <row r="97" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="97" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C97" s="3"/>
     </row>
-    <row r="98" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="98" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C98" s="3"/>
     </row>
-    <row r="99" spans="3:3" x14ac:dyDescent="0.25">
+    <row r="99" spans="3:3" x14ac:dyDescent="0.35">
       <c r="C99" s="3"/>
     </row>
   </sheetData>
@@ -2772,16 +2772,16 @@
       <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="25.28515625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="25.42578125" style="3" customWidth="1"/>
-    <col min="3" max="3" width="24.7109375" style="3" customWidth="1"/>
-    <col min="4" max="4" width="74.85546875" style="3" customWidth="1"/>
-    <col min="5" max="16384" width="9.140625" style="3"/>
+    <col min="1" max="1" width="25.26953125" style="3" customWidth="1"/>
+    <col min="2" max="2" width="25.453125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="24.7265625" style="3" customWidth="1"/>
+    <col min="4" max="4" width="74.81640625" style="3" customWidth="1"/>
+    <col min="5" max="16384" width="9.1796875" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A1" s="4" t="s">
         <v>293</v>
       </c>
@@ -2789,7 +2789,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="2" spans="1:4" ht="39.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" ht="39.5" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A2" s="16" t="s">
         <v>168</v>
       </c>
@@ -2803,7 +2803,7 @@
         <v>171</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="30.75" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" ht="29.5" thickTop="1" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
         <v>172</v>
       </c>
@@ -2814,7 +2814,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B4" s="15" t="s">
         <v>298</v>
       </c>
@@ -2825,7 +2825,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B5" s="15" t="s">
         <v>299</v>
       </c>
@@ -2836,7 +2836,7 @@
         <v>178</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
         <v>300</v>
       </c>
@@ -2847,7 +2847,7 @@
         <v>180</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
         <v>301</v>
       </c>
@@ -2858,7 +2858,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
         <v>302</v>
       </c>
@@ -2869,7 +2869,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="9" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="B9" s="15" t="s">
         <v>303</v>
       </c>
@@ -2880,7 +2880,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
         <v>304</v>
       </c>
@@ -2891,7 +2891,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="11" spans="1:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="A11" s="15" t="s">
         <v>189</v>
       </c>
@@ -2902,7 +2902,7 @@
         <v>191</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A12" s="15" t="s">
         <v>192</v>
       </c>
@@ -2913,7 +2913,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A13" s="15" t="s">
         <v>195</v>
       </c>
@@ -2924,7 +2924,7 @@
         <v>197</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="15" t="s">
         <v>198</v>
       </c>
@@ -2935,7 +2935,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="15" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A15" s="15" t="s">
         <v>201</v>
       </c>
@@ -2946,7 +2946,7 @@
         <v>203</v>
       </c>
     </row>
-    <row r="16" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A16" s="15" t="s">
         <v>204</v>
       </c>
@@ -2957,7 +2957,7 @@
         <v>206</v>
       </c>
     </row>
-    <row r="17" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B17" s="15" t="s">
         <v>305</v>
       </c>
@@ -2968,7 +2968,7 @@
         <v>208</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="B18" s="15" t="s">
         <v>306</v>
       </c>
@@ -2979,7 +2979,7 @@
         <v>210</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B19" s="15" t="s">
         <v>307</v>
       </c>
@@ -2990,7 +2990,7 @@
         <v>212</v>
       </c>
     </row>
-    <row r="20" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B20" s="15" t="s">
         <v>308</v>
       </c>
@@ -3001,7 +3001,7 @@
         <v>214</v>
       </c>
     </row>
-    <row r="21" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A21" s="15" t="s">
         <v>215</v>
       </c>
@@ -3012,7 +3012,7 @@
         <v>217</v>
       </c>
     </row>
-    <row r="22" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A22" s="15" t="s">
         <v>218</v>
       </c>
@@ -3023,7 +3023,7 @@
         <v>220</v>
       </c>
     </row>
-    <row r="23" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A23" s="15" t="s">
         <v>221</v>
       </c>
@@ -3034,7 +3034,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="24" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A24" s="15" t="s">
         <v>224</v>
       </c>
@@ -3045,7 +3045,7 @@
         <v>226</v>
       </c>
     </row>
-    <row r="25" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A25" s="15" t="s">
         <v>227</v>
       </c>
@@ -3056,7 +3056,7 @@
         <v>229</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A26" s="15" t="s">
         <v>230</v>
       </c>
@@ -3067,7 +3067,7 @@
         <v>231</v>
       </c>
     </row>
-    <row r="27" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A27" s="15" t="s">
         <v>232</v>
       </c>
@@ -3078,7 +3078,7 @@
         <v>233</v>
       </c>
     </row>
-    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A28" s="15" t="s">
         <v>234</v>
       </c>
@@ -3089,7 +3089,7 @@
         <v>236</v>
       </c>
     </row>
-    <row r="29" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A29" s="15" t="s">
         <v>237</v>
       </c>
@@ -3100,7 +3100,7 @@
         <v>238</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A30" s="15" t="s">
         <v>239</v>
       </c>
@@ -3111,7 +3111,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="31" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A31" s="15" t="s">
         <v>242</v>
       </c>
@@ -3122,7 +3122,7 @@
         <v>243</v>
       </c>
     </row>
-    <row r="32" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A32" s="15" t="s">
         <v>244</v>
       </c>
@@ -3133,7 +3133,7 @@
         <v>246</v>
       </c>
     </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A33" s="15" t="s">
         <v>247</v>
       </c>
@@ -3144,7 +3144,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="34" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A34" s="15" t="s">
         <v>250</v>
       </c>
@@ -3155,7 +3155,7 @@
         <v>251</v>
       </c>
     </row>
-    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A35" s="15" t="s">
         <v>252</v>
       </c>
@@ -3166,7 +3166,7 @@
         <v>254</v>
       </c>
     </row>
-    <row r="36" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A36" s="15" t="s">
         <v>255</v>
       </c>
@@ -3177,7 +3177,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="37" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B37" s="15" t="s">
         <v>295</v>
       </c>
@@ -3188,7 +3188,7 @@
         <v>259</v>
       </c>
     </row>
-    <row r="38" spans="1:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B38" s="15" t="s">
         <v>296</v>
       </c>
@@ -3199,7 +3199,7 @@
         <v>261</v>
       </c>
     </row>
-    <row r="39" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B39" s="15" t="s">
         <v>297</v>
       </c>
@@ -3210,7 +3210,7 @@
         <v>263</v>
       </c>
     </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A40" s="15" t="s">
         <v>264</v>
       </c>
@@ -3221,7 +3221,7 @@
         <v>265</v>
       </c>
     </row>
-    <row r="41" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A41" s="15" t="s">
         <v>59</v>
       </c>
@@ -3232,7 +3232,7 @@
         <v>267</v>
       </c>
     </row>
-    <row r="42" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="58" x14ac:dyDescent="0.35">
       <c r="A42" s="15" t="s">
         <v>61</v>
       </c>
@@ -3243,7 +3243,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="43" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A43" s="15" t="s">
         <v>62</v>
       </c>
@@ -3254,7 +3254,7 @@
         <v>270</v>
       </c>
     </row>
-    <row r="44" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A44" s="15" t="s">
         <v>271</v>
       </c>
@@ -3265,7 +3265,7 @@
         <v>273</v>
       </c>
     </row>
-    <row r="45" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A45" s="15" t="s">
         <v>274</v>
       </c>
@@ -3276,7 +3276,7 @@
         <v>276</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A46" s="15" t="s">
         <v>277</v>
       </c>
@@ -3287,7 +3287,7 @@
         <v>279</v>
       </c>
     </row>
-    <row r="47" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A47" s="15" t="s">
         <v>78</v>
       </c>
@@ -3298,7 +3298,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="48" spans="1:4" ht="60" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="A48" s="15" t="s">
         <v>281</v>
       </c>
@@ -3309,7 +3309,7 @@
         <v>282</v>
       </c>
     </row>
-    <row r="49" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A49" s="15" t="s">
         <v>283</v>
       </c>
@@ -3320,7 +3320,7 @@
         <v>284</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A50" s="15" t="s">
         <v>285</v>
       </c>
@@ -3331,7 +3331,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A51" s="15" t="s">
         <v>80</v>
       </c>
@@ -3342,7 +3342,7 @@
         <v>288</v>
       </c>
     </row>
-    <row r="52" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A52" s="15" t="s">
         <v>289</v>
       </c>
@@ -3353,7 +3353,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A53" s="15" t="s">
         <v>67</v>
       </c>

</xml_diff>

<commit_message>
rename 'identified by' to 'classification' in roles
</commit_message>
<xml_diff>
--- a/notes/vocabulary/RoleVocabulary.xlsx
+++ b/notes/vocabulary/RoleVocabulary.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Workspace\GithubC\iSamples\metadata\notes\vocabulary\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/944a82e2ddcde9eb/Documents/GithubC/iSamples/metadata/notes/vocabulary/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A07AF896-40FF-4774-8123-103315250366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="3" documentId="13_ncr:1_{A07AF896-40FF-4774-8123-103315250366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{F95C7B2D-3BC9-4DE3-BB6A-08A2FC211A2D}"/>
   <bookViews>
-    <workbookView xWindow="10485" yWindow="795" windowWidth="17235" windowHeight="15390" firstSheet="1" activeTab="4" xr2:uid="{6D09EB57-77EB-4B90-8113-743A5CC7E14E}"/>
+    <workbookView xWindow="9750" yWindow="225" windowWidth="16440" windowHeight="16455" xr2:uid="{6D09EB57-77EB-4B90-8113-743A5CC7E14E}"/>
   </bookViews>
   <sheets>
     <sheet name="SampleRelatedRoles" sheetId="3" r:id="rId1"/>
@@ -1052,9 +1052,6 @@
     <t>Agent who is responsible for making metadata public. Not necessarily the same as the agent reponsible for metadata content.</t>
   </si>
   <si>
-    <t>identified by</t>
-  </si>
-  <si>
     <t>person who assigned sample to a biological taxon or other category</t>
   </si>
   <si>
@@ -1110,6 +1107,9 @@
   </si>
   <si>
     <t>principle investigator</t>
+  </si>
+  <si>
+    <t>classification</t>
   </si>
 </sst>
 </file>
@@ -1301,6 +1301,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1602,8 +1606,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0E8140B6-11ED-4C30-ABC1-8C066247C7B6}">
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C17"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1764,10 +1768,10 @@
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
+        <v>355</v>
+      </c>
+      <c r="B16" s="3" t="s">
         <v>336</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>337</v>
       </c>
     </row>
   </sheetData>
@@ -1782,14 +1786,15 @@
   <dimension ref="A1:C22"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A23" sqref="A23"/>
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="21" customWidth="1"/>
-    <col min="2" max="2" width="61.5703125" customWidth="1"/>
-    <col min="3" max="3" width="27.28515625" customWidth="1"/>
+    <col min="1" max="1" width="21" style="4" customWidth="1"/>
+    <col min="2" max="2" width="61.5703125" style="4" customWidth="1"/>
+    <col min="3" max="3" width="27.28515625" style="4" customWidth="1"/>
+    <col min="4" max="16384" width="9.140625" style="4"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
@@ -1808,36 +1813,36 @@
         <v>8</v>
       </c>
       <c r="B2" s="3" t="s">
+        <v>341</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
+        <v>50</v>
+      </c>
+      <c r="C4" s="4" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="4" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B6" s="3" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>50</v>
-      </c>
-      <c r="C4" t="s">
-        <v>353</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" ht="30" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>53</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>343</v>
-      </c>
       <c r="C6" s="3" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
     </row>
     <row r="7" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1845,7 +1850,7 @@
         <v>330</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="C7" s="3" t="s">
         <v>314</v>
@@ -1856,10 +1861,10 @@
         <v>326</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
     </row>
     <row r="9" spans="1:3" ht="30" x14ac:dyDescent="0.25">
@@ -1867,18 +1872,18 @@
         <v>325</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" s="17" t="s">
+        <v>345</v>
+      </c>
+      <c r="C10" s="4" t="s">
         <v>346</v>
-      </c>
-      <c r="C10" t="s">
-        <v>347</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
@@ -1886,14 +1891,14 @@
         <v>329</v>
       </c>
       <c r="B11" s="3" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C11" s="3" t="s">
         <v>310</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
+      <c r="A12" s="4" t="s">
         <v>56</v>
       </c>
     </row>
@@ -1913,27 +1918,27 @@
         <v>333</v>
       </c>
       <c r="B14" s="3" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C14" s="3"/>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A15" t="s">
+      <c r="A15" s="4" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" s="17" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>354</v>
+      <c r="A17" s="4" t="s">
+        <v>353</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
+      <c r="A18" s="4" t="s">
         <v>63</v>
       </c>
     </row>
@@ -1942,25 +1947,25 @@
         <v>42</v>
       </c>
       <c r="B19" s="3" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
+      <c r="A20" s="4" t="s">
         <v>65</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
+      <c r="A21" s="4" t="s">
         <v>66</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>355</v>
+      <c r="A22" s="4" t="s">
+        <v>354</v>
       </c>
     </row>
   </sheetData>
@@ -3631,8 +3636,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19C555DF-D7F4-4F59-9A87-C7C1A37E4222}">
   <dimension ref="A9:M9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="O18" sqref="A1:O18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>